<commit_message>
Actualización de reporte de aportes
</commit_message>
<xml_diff>
--- a/Reporte de participación.xlsx
+++ b/Reporte de participación.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorburgos/Documents/GitHub/HCI-NurseCare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{472BD53B-4D70-FE42-85F7-33B427CFC610}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5474857-9D17-2348-B1A1-43B341FB824D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resúmen" sheetId="3" r:id="rId1"/>
     <sheet name="Primera Entrega" sheetId="1" r:id="rId2"/>
     <sheet name="Segunda Entrega" sheetId="2" r:id="rId3"/>
+    <sheet name="Tercera Entrega" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Resúmen!$W$15:$W$18</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Resúmen!$X$15:$X$18</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="66">
   <si>
     <t>Esthefany Geovany Mezquita Ruiz</t>
   </si>
@@ -192,13 +197,52 @@
   </si>
   <si>
     <t xml:space="preserve">Maquetar en Adobe xd </t>
+  </si>
+  <si>
+    <t>Diapositivas de la tercera entrega</t>
+  </si>
+  <si>
+    <t>Aplicar método de inspección</t>
+  </si>
+  <si>
+    <t>Ejecucion de pruebas</t>
+  </si>
+  <si>
+    <t>Elección de candidatos para pruebas</t>
+  </si>
+  <si>
+    <t>Documentación de pruebas</t>
+  </si>
+  <si>
+    <t>Analisis de resultados de las pruebas</t>
+  </si>
+  <si>
+    <t>Documento de análisis de resultados de encuestas</t>
+  </si>
+  <si>
+    <t>Creacion de prototipo interactivo</t>
+  </si>
+  <si>
+    <t>Educción por entrevistas</t>
+  </si>
+  <si>
+    <t>Revisión calendarización</t>
+  </si>
+  <si>
+    <t>Diseño + Uso de herramienta especializada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analisis + Documento </t>
+  </si>
+  <si>
+    <t>Trabajo de Campo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,11 +354,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,6 +480,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-356F-B642-A7FF-107DDA1A6197}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -451,6 +500,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-356F-B642-A7FF-107DDA1A6197}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -466,6 +520,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-356F-B642-A7FF-107DDA1A6197}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -481,6 +540,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-356F-B642-A7FF-107DDA1A6197}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -995,7 +1059,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16748548905428007"/>
+          <c:y val="0.11002160312560064"/>
+          <c:w val="0.82021984489571786"/>
+          <c:h val="0.84243979090775523"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -1040,16 +1114,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,6 +1399,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-036F-7241-9FBC-256411B080E5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1340,6 +1419,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-036F-7241-9FBC-256411B080E5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1355,6 +1439,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-036F-7241-9FBC-256411B080E5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1370,6 +1459,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-036F-7241-9FBC-256411B080E5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1398,16 +1492,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,6 +1581,359 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Aportes</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t> Etapa 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Resúmen!$W$15:$W$18</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Esthefany Geovany Mezquita Ruiz</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Luis Gerardo Vázquez Vera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hector Elias Burgos Amaya</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Erick Alberto Lechuga Torres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Resúmen!$X$15:$X$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-9817-5E44-AF40-737F24AAD5AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Resúmen!$N$16:$N$19</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Esthefany Geovany Mezquita Ruiz</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Luis Gerardo Vázquez Vera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hector Elias Burgos Amaya</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Erick Alberto Lechuga Torres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Resúmen!$O$16:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9817-5E44-AF40-737F24AAD5AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-9817-5E44-AF40-737F24AAD5AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-9817-5E44-AF40-737F24AAD5AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-9817-5E44-AF40-737F24AAD5AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-9817-5E44-AF40-737F24AAD5AC}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Resúmen!$B$17:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Esthefany Geovany Mezquita Ruiz</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Luis Gerardo Vázquez Vera</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hector Elias Burgos Amaya</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Erick Alberto Lechuga Torres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Resúmen!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-9817-5E44-AF40-737F24AAD5AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -3209,15 +3656,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:colOff>557646</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>1154</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>798946</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>94672</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3244,16 +3691,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>176646</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>207241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>278245</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>194541</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3280,16 +3727,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441325</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>106508</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:rowOff>103620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>715530</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>75045</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3309,6 +3756,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>13854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>69272</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD2E8479-3300-D544-B8A3-AD23F799B50F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3614,28 +4097,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D052903-9DE7-E64E-9CB4-152A67F50A5F}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView topLeftCell="B22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:16" ht="26">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:24" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="G2" s="11" t="s">
@@ -3651,58 +4134,72 @@
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" ht="26">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:24" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="18">
+    <row r="15" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="W15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="N16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O16">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" ht="18">
+      <c r="W16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" ht="18" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
@@ -3715,8 +4212,14 @@
       <c r="O17">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" ht="18">
+      <c r="W17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
@@ -3729,8 +4232,14 @@
       <c r="O18">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" ht="18">
+      <c r="W18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
@@ -3744,7 +4253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="18">
+    <row r="20" spans="2:24" ht="18" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>4</v>
       </c>
@@ -3752,40 +4261,36 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="7:8" ht="18">
+    <row r="35" spans="7:8" ht="18" x14ac:dyDescent="0.2">
       <c r="G35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="H35">
-        <f>SUM(C17,O16)</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="7:8" ht="18">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" ht="18" x14ac:dyDescent="0.2">
       <c r="G36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H36">
-        <f>SUM(C18,O17)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="7:8" ht="18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" ht="18" x14ac:dyDescent="0.2">
       <c r="G37" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H37">
-        <f>SUM(C19,O18)</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="7:8" ht="18">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" ht="18" x14ac:dyDescent="0.2">
       <c r="G38" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H38">
-        <f>SUM(C20,O19)</f>
-        <v>64</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3802,11 +4307,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FD23A2-AC58-E546-AB1C-AB7E9032A481}">
   <dimension ref="A4:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" customWidth="1"/>
@@ -3818,12 +4323,12 @@
     <col min="10" max="10" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="29">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
@@ -3837,7 +4342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -3857,7 +4362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3877,7 +4382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3897,7 +4402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3917,7 +4422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
         <v>25</v>
       </c>
@@ -3928,7 +4433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -3937,7 +4442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H17" t="s">
         <v>28</v>
       </c>
@@ -3946,7 +4451,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="18">
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
@@ -3960,7 +4465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -3980,7 +4485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -4000,7 +4505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -4020,7 +4525,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -4040,7 +4545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>28</v>
       </c>
@@ -4065,11 +4570,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40D257C-314C-C240-8BD9-5922FF652990}">
   <dimension ref="A4:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.33203125" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" customWidth="1"/>
@@ -4079,12 +4584,12 @@
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="29">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
@@ -4098,7 +4603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4118,7 +4623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -4138,7 +4643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -4158,7 +4663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -4178,7 +4683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -4198,7 +4703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -4214,7 +4719,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="18">
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
@@ -4228,7 +4733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -4248,7 +4753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -4268,7 +4773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -4288,7 +4793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -4308,7 +4813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -4328,7 +4833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -4348,7 +4853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>28</v>
       </c>
@@ -4357,13 +4862,295 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H35" t="s">
         <v>28</v>
       </c>
       <c r="I35">
         <f>SUM(I28:I34)</f>
         <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2FC6C8-4ADF-9E41-9B1E-65FEBA4FAC82}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="39.5" customWidth="1"/>
+    <col min="7" max="7" width="46.33203125" customWidth="1"/>
+    <col min="8" max="8" width="37.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C9:C13)</f>
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14">
+        <f>SUM(I9:I12)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="I28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <f>SUM(C25:C29)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32">
+        <f>SUM(I25:I31)</f>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se eliminaron archivos basura
</commit_message>
<xml_diff>
--- a/Reporte de participación.xlsx
+++ b/Reporte de participación.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorburgos/Documents/GitHub/HCI-NurseCare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorburgos/Documents/HCI-NurseCare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5474857-9D17-2348-B1A1-43B341FB824D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B305C5-A499-BF40-BE62-8AC0131303C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="3" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resúmen" sheetId="3" r:id="rId1"/>
@@ -18,10 +18,6 @@
     <sheet name="Segunda Entrega" sheetId="2" r:id="rId3"/>
     <sheet name="Tercera Entrega" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Resúmen!$W$15:$W$18</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Resúmen!$X$15:$X$18</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="67">
   <si>
     <t>Esthefany Geovany Mezquita Ruiz</t>
   </si>
@@ -236,6 +232,9 @@
   </si>
   <si>
     <t>Trabajo de Campo</t>
+  </si>
+  <si>
+    <t>Planeación de proyecto NurseCare Etapa 3 - tercera entrega</t>
   </si>
 </sst>
 </file>
@@ -4881,7 +4880,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4894,7 +4893,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="C1" s="7" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Actualización de actividades asignadas
</commit_message>
<xml_diff>
--- a/Reporte de participación.xlsx
+++ b/Reporte de participación.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorburgos/Documents/HCI-NurseCare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorburgos/Git/HCI-NurseCare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B305C5-A499-BF40-BE62-8AC0131303C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360FF6F2-394D-1C42-A4F1-7173940C727E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="3" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resúmen" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="71">
   <si>
     <t>Esthefany Geovany Mezquita Ruiz</t>
   </si>
@@ -195,9 +195,6 @@
     <t xml:space="preserve">Maquetar en Adobe xd </t>
   </si>
   <si>
-    <t>Diapositivas de la tercera entrega</t>
-  </si>
-  <si>
     <t>Aplicar método de inspección</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>Elección de candidatos para pruebas</t>
   </si>
   <si>
-    <t>Documentación de pruebas</t>
-  </si>
-  <si>
     <t>Analisis de resultados de las pruebas</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Educción por entrevistas</t>
   </si>
   <si>
-    <t>Revisión calendarización</t>
-  </si>
-  <si>
     <t>Diseño + Uso de herramienta especializada</t>
   </si>
   <si>
@@ -235,6 +226,27 @@
   </si>
   <si>
     <t>Planeación de proyecto NurseCare Etapa 3 - tercera entrega</t>
+  </si>
+  <si>
+    <t>Realizó Poster</t>
+  </si>
+  <si>
+    <t>Realizó artículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creación de video </t>
+  </si>
+  <si>
+    <t>Revisión de documentos y calendarización</t>
+  </si>
+  <si>
+    <t>Herramienta especializada + Diseño  + Documento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de herramienta especializada + analisis + diseño + documento  </t>
+  </si>
+  <si>
+    <t>Documento + analisis+diseño + investigación</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1075,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16748548905428007"/>
-          <c:y val="0.11002160312560064"/>
+          <c:x val="0.15668108555579341"/>
+          <c:y val="0.109999995884335"/>
           <c:w val="0.82021984489571786"/>
           <c:h val="0.84243979090775523"/>
         </c:manualLayout>
@@ -1113,16 +1125,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>112</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1491,16 +1503,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>112</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1686,16 +1698,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3619,15 +3631,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1930400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>669636</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>92364</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>319809</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>16164</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3654,16 +3666,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>557646</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1154</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>185880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>798946</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>94672</xdr:rowOff>
+      <xdr:colOff>210128</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>71580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3690,16 +3702,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>176646</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>207241</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>684645</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>10968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>278245</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>194541</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>786245</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>206086</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3726,16 +3738,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>106508</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>103620</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>348962</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>207528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>715530</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>75045</xdr:rowOff>
+      <xdr:colOff>126712</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>178952</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3763,15 +3775,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>13854</xdr:rowOff>
+      <xdr:colOff>398317</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>13855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>69272</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>658089</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>69274</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4098,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D052903-9DE7-E64E-9CB4-152A67F50A5F}">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4181,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="X15">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="18" x14ac:dyDescent="0.2">
@@ -4195,7 +4207,7 @@
         <v>5</v>
       </c>
       <c r="X16">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:24" ht="18" x14ac:dyDescent="0.2">
@@ -4215,7 +4227,7 @@
         <v>6</v>
       </c>
       <c r="X17">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:24" ht="18" x14ac:dyDescent="0.2">
@@ -4235,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="X18">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:24" ht="18" x14ac:dyDescent="0.2">
@@ -4265,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="7:8" ht="18" x14ac:dyDescent="0.2">
@@ -4273,7 +4285,7 @@
         <v>5</v>
       </c>
       <c r="H36">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="7:8" ht="18" x14ac:dyDescent="0.2">
@@ -4281,7 +4293,7 @@
         <v>6</v>
       </c>
       <c r="H37">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="7:8" ht="18" x14ac:dyDescent="0.2">
@@ -4289,7 +4301,7 @@
         <v>4</v>
       </c>
       <c r="H38">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4569,7 +4581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40D257C-314C-C240-8BD9-5922FF652990}">
   <dimension ref="A4:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -4879,8 +4891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2FC6C8-4ADF-9E41-9B1E-65FEBA4FAC82}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4893,7 +4905,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="C1" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -4932,7 +4944,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -4941,10 +4953,10 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I9">
         <v>11</v>
@@ -4972,19 +4984,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I11">
         <v>11</v>
@@ -4992,13 +5004,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
         <v>38</v>
@@ -5010,20 +5022,51 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f>SUM(C9:C13)</f>
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
         <v>28</v>
       </c>
-      <c r="I14">
-        <f>SUM(I9:I12)</f>
-        <v>44</v>
+      <c r="I15">
+        <f>SUM(I9:I14)</f>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -5071,7 +5114,7 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="H25" t="s">
         <v>42</v>
@@ -5082,19 +5125,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
       </c>
       <c r="C26">
         <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I26">
         <v>10</v>
@@ -5102,16 +5145,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C27">
         <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H27" t="s">
         <v>42</v>
@@ -5122,16 +5165,42 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>11</v>
       </c>
-      <c r="I28">
-        <v>6</v>
+      <c r="G29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -5140,7 +5209,7 @@
       </c>
       <c r="C31">
         <f>SUM(C25:C29)</f>
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5148,8 +5217,7 @@
         <v>28</v>
       </c>
       <c r="I32">
-        <f>SUM(I25:I31)</f>
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Reporte de participación.xlsx
</commit_message>
<xml_diff>
--- a/Reporte de participación.xlsx
+++ b/Reporte de participación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectorburgos/Git/HCI-NurseCare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360FF6F2-394D-1C42-A4F1-7173940C727E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC7E08F-D164-C64A-AA27-0E847CC11D1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="3" xr2:uid="{D975643D-C63E-1946-8FA5-6255F0E0328A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resúmen" sheetId="3" r:id="rId1"/>
@@ -3739,13 +3739,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>348962</xdr:colOff>
+      <xdr:colOff>672235</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>207528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>126712</xdr:colOff>
+      <xdr:colOff>449985</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>178952</xdr:rowOff>
     </xdr:to>
@@ -4110,7 +4110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D052903-9DE7-E64E-9CB4-152A67F50A5F}">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -4891,7 +4891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2FC6C8-4ADF-9E41-9B1E-65FEBA4FAC82}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>